<commit_message>
complete element logic, refactor main modules
</commit_message>
<xml_diff>
--- a/data/Projects.xlsx
+++ b/data/Projects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_work\Projects\ProjectManagerDemo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB822A58-B28F-410F-98CD-425545F8F53D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0EFB73-B7FB-4CC1-9FE2-FF0526B457FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8580" yWindow="900" windowWidth="18510" windowHeight="16290" xr2:uid="{03501B73-0365-4973-85A8-AB612169F046}"/>
+    <workbookView xWindow="29580" yWindow="780" windowWidth="20280" windowHeight="13875" xr2:uid="{03501B73-0365-4973-85A8-AB612169F046}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,15 +47,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>ClientID</t>
-  </si>
-  <si>
-    <t>ProjectTypeID</t>
-  </si>
-  <si>
-    <t>EmployeeCode</t>
-  </si>
-  <si>
     <t>AccountingName</t>
   </si>
   <si>
@@ -147,6 +138,15 @@
   </si>
   <si>
     <t>PR02</t>
+  </si>
+  <si>
+    <t>ClientId</t>
+  </si>
+  <si>
+    <t>ProjectTypeId</t>
+  </si>
+  <si>
+    <t>EmployeeId</t>
   </si>
 </sst>
 </file>
@@ -521,7 +521,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,137 +544,236 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>11</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>11</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>22</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>11</v>
+      </c>
+      <c r="F12">
+        <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>